<commit_message>
Aggiunti attributi al file Auto
</commit_message>
<xml_diff>
--- a/db-first-auto.xlsx
+++ b/db-first-auto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Downloads\NotOneDrive\EserciziGIT\db-first\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECD89EB8-EF66-4F52-8387-5024F3ACA53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{CD843736-5227-4989-A119-E500B749CA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -108,13 +108,25 @@
   </si>
   <si>
     <t>Considerazione sugli ENUM: Queste possono essere anche CHAR o TINYINT, ma la costruzione delle auto segue determinati criteri. Il motore può essere a benzina, diesel, GPL o elettrico; altri valori non dovrebbero essere ammessi (salvo eccezioni, al massimo)</t>
+  </si>
+  <si>
+    <t>NOTNULL</t>
+  </si>
+  <si>
+    <t>IDENTITY, UNIQUE</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +136,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -268,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -314,6 +334,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -629,15 +655,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
@@ -646,8 +672,8 @@
     <col min="8" max="8" width="15.140625" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
     <col min="13" max="13" width="13.42578125" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" customWidth="1"/>
   </cols>
@@ -740,65 +766,158 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="3"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="3"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="12"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="12"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="13"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="H4:L7"/>
+  <mergeCells count="3">
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="H8:L11"/>
+    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correzioni all'esercizio delle auto
</commit_message>
<xml_diff>
--- a/db-first-auto.xlsx
+++ b/db-first-auto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Downloads\NotOneDrive\EserciziGIT\db-first\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{CD843736-5227-4989-A119-E500B749CA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{E4B50937-A8F3-408E-BE12-9DD04B80A91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -119,7 +119,16 @@
     <t>UNIQUE</t>
   </si>
   <si>
-    <t>DEFAULT</t>
+    <t>DEFAULT(0)</t>
+  </si>
+  <si>
+    <t>DEFAULT(false)</t>
+  </si>
+  <si>
+    <t>Chiave primaria</t>
+  </si>
+  <si>
+    <t>(Riprendo dalla mia conoscenza degli enum su Unity) I campi enum non possono essere lasciati a null: se non specificati defaultano al primo valore. Da non fare, ma almeno si evita il crash del programma.</t>
   </si>
 </sst>
 </file>
@@ -288,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,6 +349,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -655,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +716,7 @@
     <col min="10" max="10" width="11.85546875" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -751,7 +793,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>20</v>
@@ -794,7 +836,9 @@
       <c r="I3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="16"/>
+      <c r="J3" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="K3" s="16" t="s">
         <v>24</v>
       </c>
@@ -802,7 +846,7 @@
         <v>24</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N3" s="16" t="s">
         <v>24</v>
@@ -818,11 +862,21 @@
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
+      <c r="H4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>27</v>
+      </c>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
     </row>
@@ -843,7 +897,9 @@
       <c r="N5" s="16"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="26" t="s">
+        <v>29</v>
+      </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -858,39 +914,29 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22"/>
+    </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="24"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="8" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="12"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="10"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -900,24 +946,64 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="11"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="12"/>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H11" s="13"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="12"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="13"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="20"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H14" s="27"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="28"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="21"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="H8:L11"/>
+  <mergeCells count="5">
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="H9:L12"/>
     <mergeCell ref="A3:A5"/>
+    <mergeCell ref="H13:L15"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>